<commit_message>
Misc files I forgot to commit.
</commit_message>
<xml_diff>
--- a/PII/test_PII_regexner.xlsx
+++ b/PII/test_PII_regexner.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="900" windowWidth="20490" windowHeight="6465"/>
+    <workbookView xWindow="0" yWindow="1350" windowWidth="20490" windowHeight="6465"/>
   </bookViews>
   <sheets>
     <sheet name="test_PII_regexner" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">test_PII_regexner!$A$1:$H$138</definedName>
   </definedNames>
-  <calcPr calcId="0"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
@@ -1314,7 +1314,7 @@
   <dimension ref="A1:I138"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="I42" sqref="I42"/>
+      <selection activeCell="I45" sqref="I45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>